<commit_message>
changed internal battery measurement
</commit_message>
<xml_diff>
--- a/calc fact for battery class.xlsx
+++ b/calc fact for battery class.xlsx
@@ -71,7 +71,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -120,7 +120,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -468,7 +468,7 @@
   <dimension ref="B2:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -548,7 +548,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="5">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="2:8">
@@ -572,7 +572,7 @@
       </c>
       <c r="F13" s="2">
         <f>F10*F12</f>
-        <v>283.87096774193549</v>
+        <v>286.02150537634407</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>6</v>
@@ -589,7 +589,7 @@
       </c>
       <c r="F16" s="5">
         <f>F2/F10*10</f>
-        <v>121.21212121212122</v>
+        <v>120.30075187969925</v>
       </c>
       <c r="H16" s="2">
         <f>F10/10*F16</f>
@@ -606,7 +606,7 @@
       </c>
       <c r="H17" s="2">
         <f>ROUND(F10/10,0)*F17</f>
-        <v>3224</v>
+        <v>3348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>